<commit_message>
Updating MentorPAL to latest PAL3 version
</commit_message>
<xml_diff>
--- a/mentors/clint/data/Prompts_Utterances.xlsx
+++ b/mentors/clint/data/Prompts_Utterances.xlsx
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>